<commit_message>
adjusted class diagramm and rest spec
</commit_message>
<xml_diff>
--- a/rest_specification.xlsx
+++ b/rest_specification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bara1\OneDrive\Documents\Daten\Studium\4. Semester\SoPra\Assignments\Assignment_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bara1\Documents\Uni Code Repos\SoPra_2022\roomeight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{22A6084C-F823-4533-BF96-C27AE24E1440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51ACF0C4-33A6-4983-951E-BB67AC3BA7E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1D422A-EF40-472B-AC1F-1D1159984CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="366" yWindow="366" windowWidth="17280" windowHeight="8994" xr2:uid="{AB8D1724-D936-40B2-B7D4-F42EB9C9C2A8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AB8D1724-D936-40B2-B7D4-F42EB9C9C2A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="76">
   <si>
     <t xml:space="preserve">Data Service </t>
   </si>
@@ -64,48 +64,21 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Login/Logout</t>
-  </si>
-  <si>
-    <t>/login</t>
-  </si>
-  <si>
     <t>post</t>
   </si>
   <si>
     <t>body</t>
   </si>
   <si>
-    <t>email, password</t>
-  </si>
-  <si>
     <t>User Profile</t>
   </si>
   <si>
-    <t>Login User</t>
-  </si>
-  <si>
     <t>error</t>
   </si>
   <si>
-    <t>Login User with invalid credentials</t>
-  </si>
-  <si>
-    <t>/logout</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
-    <t>"Successfully loged out"</t>
-  </si>
-  <si>
-    <t>Logout User</t>
-  </si>
-  <si>
-    <t>Logout User with invalid auth</t>
-  </si>
-  <si>
     <t>User Profile Operations</t>
   </si>
   <si>
@@ -232,9 +205,6 @@
     <t>Profile Operations</t>
   </si>
   <si>
-    <t>/profile?id={id}</t>
-  </si>
-  <si>
     <t>Profile</t>
   </si>
   <si>
@@ -247,9 +217,6 @@
     <t>Get Profile by Id but profile not found</t>
   </si>
   <si>
-    <t>/profile/filter</t>
-  </si>
-  <si>
     <t>Filter List</t>
   </si>
   <si>
@@ -265,9 +232,6 @@
     <t>Get Profile by Filters but invalid Filters</t>
   </si>
   <si>
-    <t>/profile/matches</t>
-  </si>
-  <si>
     <t>Get Matches by Id</t>
   </si>
   <si>
@@ -277,9 +241,6 @@
     <t>Get Matches by Id but profile not found</t>
   </si>
   <si>
-    <t>/profile/match</t>
-  </si>
-  <si>
     <t>UserId, MatchId</t>
   </si>
   <si>
@@ -290,13 +251,25 @@
   </si>
   <si>
     <t>Match a profile but profile not found</t>
+  </si>
+  <si>
+    <t>/profiles?id={id}</t>
+  </si>
+  <si>
+    <t>/profiles/filter</t>
+  </si>
+  <si>
+    <t>/profiles/matches</t>
+  </si>
+  <si>
+    <t>/profiles/match</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,7 +534,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -859,11 +832,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0F73B0-48B0-4C85-A0C8-1E6762A3CC0A}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -874,12 +847,12 @@
     <col min="8" max="8" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -905,926 +878,829 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="F4">
-        <v>200</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E9" t="s">
         <v>13</v>
-      </c>
-      <c r="F5">
-        <v>401</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6">
-        <v>200</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>403</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
       </c>
       <c r="F9">
         <v>200</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>403</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
       </c>
       <c r="F11">
         <v>201</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
       </c>
       <c r="F12">
         <v>403</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
         <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
       </c>
       <c r="F13">
         <v>400</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
         <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
       </c>
       <c r="F14">
         <v>200</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>33</v>
       </c>
       <c r="F15">
         <v>403</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
         <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
       </c>
       <c r="F16">
         <v>404</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
         <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
       </c>
       <c r="F17">
         <v>400</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F18">
         <v>200</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F19">
         <v>403</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F20">
         <v>404</v>
       </c>
       <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="H20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>200</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F23">
         <v>403</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F24">
         <v>201</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F25">
         <v>403</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F26">
         <v>400</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F27">
         <v>200</v>
       </c>
       <c r="G27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F28">
         <v>403</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F29">
         <v>404</v>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F30">
         <v>400</v>
       </c>
       <c r="G30" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F31">
         <v>200</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F32">
         <v>403</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F33">
         <v>404</v>
       </c>
       <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="H33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>25</v>
-      </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F35">
         <v>200</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F36">
         <v>403</v>
       </c>
       <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="H36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>25</v>
-      </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F37">
         <v>404</v>
       </c>
       <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" t="s">
         <v>16</v>
       </c>
-      <c r="H37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" t="s">
-        <v>25</v>
-      </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F38">
         <v>200</v>
       </c>
       <c r="G38" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F39">
         <v>403</v>
       </c>
       <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
         <v>16</v>
       </c>
-      <c r="H39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" t="s">
-        <v>25</v>
-      </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F40">
         <v>400</v>
       </c>
       <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
         <v>16</v>
       </c>
-      <c r="H40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" t="s">
-        <v>25</v>
-      </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E41" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F41">
         <v>200</v>
       </c>
       <c r="H41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E42" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F42">
         <v>403</v>
       </c>
       <c r="H42" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F43">
         <v>404</v>
       </c>
       <c r="H43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F44">
         <v>200</v>
       </c>
       <c r="H44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F45">
         <v>403</v>
       </c>
       <c r="H45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F46">
         <v>404</v>
       </c>
       <c r="H46" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1983,13 +1859,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FA7B352-9218-4F50-810D-6EC6BA654247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FA7B352-9218-4F50-810D-6EC6BA654247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3001D0B6-1FC3-4E51-ACE8-B730309B2008}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3001D0B6-1FC3-4E51-ACE8-B730309B2008}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c5bf38a-4488-4be4-b211-4cdefd00800a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB6E6E88-C173-4671-A7A6-FF0F193E3964}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB6E6E88-C173-4671-A7A6-FF0F193E3964}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>